<commit_message>
update test description and data.
</commit_message>
<xml_diff>
--- a/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
+++ b/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\API-test-collection\exam-API-test\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941C4CD-2749-4E21-9D9F-BF99F74F33F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D17DC4-E342-4BB8-8A1B-DC285832ADBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11235" xr2:uid="{9860E287-64AD-465F-86C0-8AA7A7BCB37D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9860E287-64AD-465F-86C0-8AA7A7BCB37D}"/>
   </bookViews>
   <sheets>
     <sheet name="exam.cases.TestNewExamPaper" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>paperId</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,10 @@
   </si>
   <si>
     <t>testDeleteNewExamPaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testAddNewExamPaper</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,14 +470,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23502096-395D-4683-9EB8-8BD292EB1D31}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -489,7 +494,7 @@
     </row>
     <row r="2" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
fix create position authentication case, and refactor get resourece file stream method.
</commit_message>
<xml_diff>
--- a/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
+++ b/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\API-test-collection\exam-API-test\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D17DC4-E342-4BB8-8A1B-DC285832ADBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A0A26-B307-4BBD-B5CE-5AB45519008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9860E287-64AD-465F-86C0-8AA7A7BCB37D}"/>
   </bookViews>
@@ -39,14 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Automation1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Automation2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>papeTitle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,6 +75,14 @@
   </si>
   <si>
     <t>testAddNewExamPaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automation001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automation002</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,7 +471,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -482,88 +482,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
+      <c r="A9" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update case of new exam into newexam package.
</commit_message>
<xml_diff>
--- a/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
+++ b/exam-API-test/src/test/resources/testdata/TestNewExamPaperData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\API-test-collection\exam-API-test\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390A0A26-B307-4BBD-B5CE-5AB45519008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8B1E72-3C3A-4395-8363-8BD47EEEC3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9860E287-64AD-465F-86C0-8AA7A7BCB37D}"/>
   </bookViews>
   <sheets>
-    <sheet name="exam.cases.TestNewExamPaper" sheetId="1" r:id="rId1"/>
+    <sheet name="newexam.cases.TestNewExamPaper" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -471,7 +471,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>